<commit_message>
Changes to Project Files
</commit_message>
<xml_diff>
--- a/data/raw/2018Girls Rock Data Analysis.xlsx
+++ b/data/raw/2018Girls Rock Data Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unomail-my.sharepoint.com/personal/joshellis_unomaha_edu/Documents/COURSES/FALL_2022/ISQA8156-820/course-project/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{9329157D-59F7-3E41-B9DD-31257E0B7100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FD8FEF1-41BA-4BC0-AFCD-0306153E6469}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{9329157D-59F7-3E41-B9DD-31257E0B7100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BDB69C0-832F-49AC-998B-EA13C779BF20}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PREtest-Older Group" sheetId="4" r:id="rId1"/>
@@ -19653,8 +19653,8 @@
   </sheetPr>
   <dimension ref="A1:AH155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AG4" sqref="AG4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19679,11 +19679,11 @@
     <col min="22" max="22" width="15.42578125" customWidth="1"/>
     <col min="23" max="23" width="15.85546875" customWidth="1"/>
     <col min="24" max="24" width="15.140625" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" customWidth="1"/>
+    <col min="25" max="25" width="15.28515625" customWidth="1"/>
+    <col min="26" max="26" width="17.7109375" customWidth="1"/>
     <col min="27" max="27" width="15.42578125" customWidth="1"/>
     <col min="28" max="28" width="13.42578125" customWidth="1"/>
-    <col min="29" max="29" width="12.7109375" customWidth="1"/>
+    <col min="29" max="29" width="17.28515625" customWidth="1"/>
     <col min="30" max="30" width="15.42578125" style="1" customWidth="1"/>
     <col min="31" max="31" width="14.42578125" style="3" customWidth="1"/>
     <col min="32" max="32" width="12.42578125" style="3" customWidth="1"/>
@@ -27551,7 +27551,7 @@
   </sheetPr>
   <dimension ref="A1:AH236"/>
   <sheetViews>
-    <sheetView topLeftCell="S38" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="AH51" sqref="AH51"/>
     </sheetView>
   </sheetViews>

</xml_diff>